<commit_message>
BP8 heater rev 2
</commit_message>
<xml_diff>
--- a/BP8/Heater/PCB_ordering_document.xlsx
+++ b/BP8/Heater/PCB_ordering_document.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="Denne_projektmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mogn\Documents\GitHub\Hardware\nanopower\P80\BP8\Heater\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mogn\Documents\GitHub\Hardware\nanopower\BP8\Heater\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'PCB Specifications'!$B$2:$H$56</definedName>
     <definedName name="R_">'PCB Specifications'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -309,9 +309,6 @@
     <t>NanoPower BP8 Heater</t>
   </si>
   <si>
-    <t>Top layer 150 ohm +/- 3%</t>
-  </si>
-  <si>
     <t>Two layer flex</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>Flex_heater_default.GCT2</t>
+  </si>
+  <si>
+    <t>Top layer 150 ohm +/- 5%</t>
   </si>
 </sst>
 </file>
@@ -990,14 +990,83 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1005,41 +1074,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1047,68 +1086,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1118,24 +1103,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1210,72 +1177,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1283,6 +1184,105 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6309,7 +6309,7 @@
   </sheetPr>
   <dimension ref="A1:Q334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G33" sqref="G33:H33"/>
     </sheetView>
   </sheetViews>
@@ -6333,159 +6333,159 @@
       <c r="K1" s="47"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="85"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126"/>
       <c r="E2" s="30"/>
       <c r="F2" s="29"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="122"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="88"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="31"/>
       <c r="F3" s="27"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="81"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="123"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="31"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="81"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="123"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="132"/>
       <c r="E5" s="31"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="123"/>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="94"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="135"/>
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
       <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="95"/>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="97"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="140"/>
-      <c r="C8" s="143" t="s">
+      <c r="B8" s="63"/>
+      <c r="C8" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="146">
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="70">
         <f ca="1">TODAY()</f>
-        <v>43185</v>
+        <v>43405</v>
       </c>
-      <c r="H8" s="72"/>
+      <c r="H8" s="71"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="141"/>
-      <c r="C9" s="144" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="144"/>
-      <c r="E9" s="144"/>
-      <c r="F9" s="145"/>
-      <c r="G9" s="147" t="s">
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="148"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="141"/>
-      <c r="C10" s="143" t="s">
+      <c r="B10" s="64"/>
+      <c r="C10" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="143"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="64">
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="74">
         <v>102477</v>
       </c>
-      <c r="H10" s="72"/>
+      <c r="H10" s="71"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="141"/>
-      <c r="C11" s="144" t="s">
+      <c r="B11" s="64"/>
+      <c r="C11" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="144"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="145"/>
-      <c r="G11" s="147">
-        <v>1</v>
-      </c>
-      <c r="H11" s="148"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="141"/>
-      <c r="C12" s="143" t="s">
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="72">
         <v>2</v>
       </c>
-      <c r="D12" s="143"/>
-      <c r="E12" s="143"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="64" t="s">
+      <c r="H11" s="73"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="64"/>
+      <c r="C12" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="72"/>
+      <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="141"/>
-      <c r="C13" s="66" t="s">
+      <c r="B13" s="64"/>
+      <c r="C13" s="147" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="148"/>
     </row>
     <row r="14" spans="1:17" s="44" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="43"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="68" t="s">
+      <c r="B14" s="64"/>
+      <c r="C14" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="129" t="s">
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="130"/>
+      <c r="H14" s="79"/>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
       <c r="K14" s="47"/>
@@ -6495,71 +6495,71 @@
       <c r="O14" s="43"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="141"/>
-      <c r="C15" s="70" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59" t="s">
-        <v>83</v>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60" t="s">
+        <v>82</v>
       </c>
-      <c r="H15" s="71"/>
+      <c r="H15" s="77"/>
       <c r="Q15" s="14"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="141"/>
-      <c r="C16" s="65" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64" t="s">
-        <v>82</v>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74" t="s">
+        <v>81</v>
       </c>
-      <c r="H16" s="72"/>
+      <c r="H16" s="71"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="141"/>
-      <c r="C17" s="70" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59">
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60">
         <v>2</v>
       </c>
-      <c r="H17" s="71"/>
+      <c r="H17" s="77"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="141"/>
-      <c r="C18" s="65" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="149" t="s">
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="150"/>
+      <c r="H18" s="76"/>
     </row>
     <row r="19" spans="1:15" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
-      <c r="B19" s="142"/>
-      <c r="C19" s="70" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="134" t="s">
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="135"/>
+      <c r="H19" s="62"/>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="47"/>
@@ -6570,15 +6570,15 @@
     </row>
     <row r="20" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="75"/>
+      <c r="C20" s="152"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="153"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="47"/>
@@ -6590,16 +6590,16 @@
     <row r="21" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64" t="s">
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="72"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="47"/>
@@ -6611,16 +6611,16 @@
     <row r="22" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59" t="s">
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="71"/>
+      <c r="H22" s="77"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="47"/>
@@ -6632,16 +6632,16 @@
     <row r="23" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64" t="s">
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="72"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="47"/>
@@ -6653,16 +6653,16 @@
     <row r="24" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59" t="s">
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="71"/>
+      <c r="H24" s="77"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="47"/>
@@ -6674,16 +6674,16 @@
     <row r="25" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64" t="s">
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="72"/>
+      <c r="H25" s="71"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="47"/>
@@ -6695,16 +6695,16 @@
     <row r="26" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59" t="s">
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="71"/>
+      <c r="H26" s="77"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="47"/>
@@ -6716,16 +6716,16 @@
     <row r="27" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="60" t="s">
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="61"/>
+      <c r="H27" s="146"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="47"/>
@@ -6737,16 +6737,16 @@
     <row r="28" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="62" t="s">
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="63"/>
+      <c r="H28" s="86"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="47"/>
@@ -6758,16 +6758,16 @@
     <row r="29" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="60" t="s">
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="145" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="61"/>
+      <c r="H29" s="146"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="46"/>
@@ -6779,16 +6779,16 @@
     <row r="30" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="138" t="s">
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="71"/>
+      <c r="H30" s="77"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="46"/>
@@ -6800,16 +6800,16 @@
     <row r="31" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="76" t="s">
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="77"/>
+      <c r="H31" s="90"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
       <c r="K31" s="46"/>
@@ -6821,16 +6821,16 @@
     <row r="32" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28"/>
       <c r="B32" s="48"/>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="138" t="s">
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="139"/>
+      <c r="H32" s="88"/>
       <c r="I32" s="42"/>
       <c r="J32" s="42"/>
       <c r="K32" s="46"/>
@@ -6842,16 +6842,16 @@
     <row r="33" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28"/>
       <c r="B33" s="41"/>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="76" t="s">
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="H33" s="77"/>
+      <c r="H33" s="90"/>
       <c r="I33" s="40"/>
       <c r="J33" s="40"/>
       <c r="K33" s="46"/>
@@ -6863,16 +6863,16 @@
     <row r="34" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28"/>
       <c r="B34" s="48"/>
-      <c r="C34" s="62" t="s">
+      <c r="C34" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="102"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="134" t="s">
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="135"/>
+      <c r="H34" s="62"/>
       <c r="I34" s="40"/>
       <c r="J34" s="40"/>
       <c r="K34" s="46"/>
@@ -6884,14 +6884,14 @@
     <row r="35" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28"/>
       <c r="B35" s="41"/>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="136"/>
-      <c r="H35" s="137"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="84"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
       <c r="K35" s="46"/>
@@ -6903,16 +6903,16 @@
     <row r="36" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25"/>
       <c r="B36" s="48"/>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="62" t="s">
-        <v>81</v>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="85" t="s">
+        <v>96</v>
       </c>
-      <c r="H36" s="63"/>
+      <c r="H36" s="86"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
       <c r="K36" s="46"/>
@@ -6924,16 +6924,16 @@
     <row r="37" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28"/>
       <c r="B37" s="41"/>
-      <c r="C37" s="64" t="s">
+      <c r="C37" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="136" t="s">
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="137"/>
+      <c r="H37" s="84"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
       <c r="K37" s="46"/>
@@ -6944,15 +6944,15 @@
     </row>
     <row r="38" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="28"/>
-      <c r="B38" s="131" t="s">
+      <c r="B38" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="132"/>
-      <c r="D38" s="132"/>
-      <c r="E38" s="132"/>
-      <c r="F38" s="132"/>
-      <c r="G38" s="132"/>
-      <c r="H38" s="133"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="81"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="82"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
       <c r="K38" s="46"/>
@@ -6963,11 +6963,11 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B39" s="37"/>
-      <c r="C39" s="103" t="s">
+      <c r="C39" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="104"/>
-      <c r="E39" s="105"/>
+      <c r="D39" s="142"/>
+      <c r="E39" s="143"/>
       <c r="F39" s="38" t="s">
         <v>4</v>
       </c>
@@ -6984,11 +6984,11 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B40" s="35"/>
-      <c r="C40" s="106" t="s">
+      <c r="C40" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="106"/>
-      <c r="E40" s="106"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="144"/>
       <c r="F40" s="50" t="s">
         <v>11</v>
       </c>
@@ -7005,16 +7005,16 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="107" t="s">
+      <c r="C41" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="107"/>
-      <c r="E41" s="107"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
       <c r="F41" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G41" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>10</v>
@@ -7026,16 +7026,16 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
-      <c r="C42" s="99" t="s">
+      <c r="C42" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="100"/>
-      <c r="E42" s="101"/>
+      <c r="D42" s="95"/>
+      <c r="E42" s="96"/>
       <c r="F42" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H42" s="15" t="s">
         <v>68</v>
@@ -7047,16 +7047,16 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
-      <c r="C43" s="107" t="s">
+      <c r="C43" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="107"/>
-      <c r="E43" s="107"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="93"/>
       <c r="F43" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43" s="57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H43" s="16" t="s">
         <v>69</v>
@@ -7068,19 +7068,19 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B44" s="8"/>
-      <c r="C44" s="98" t="s">
-        <v>84</v>
+      <c r="C44" s="139" t="s">
+        <v>83</v>
       </c>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="139"/>
       <c r="F44" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H44" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="27"/>
@@ -7089,16 +7089,16 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B45" s="53"/>
-      <c r="C45" s="126" t="s">
+      <c r="C45" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="127"/>
-      <c r="E45" s="128"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="117"/>
       <c r="F45" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G45" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>70</v>
@@ -7107,16 +7107,16 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B46" s="41"/>
-      <c r="C46" s="151" t="s">
+      <c r="C46" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="152"/>
-      <c r="E46" s="153"/>
+      <c r="D46" s="119"/>
+      <c r="E46" s="120"/>
       <c r="F46" s="58" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G46" s="58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>71</v>
@@ -7125,30 +7125,30 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B47" s="53"/>
-      <c r="C47" s="126" t="s">
+      <c r="C47" s="115" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="116"/>
+      <c r="E47" s="117"/>
+      <c r="F47" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="127"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="54" t="s">
-        <v>88</v>
-      </c>
       <c r="H47" s="56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="8"/>
-      <c r="C48" s="99" t="s">
+      <c r="C48" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="100"/>
-      <c r="E48" s="101"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="96"/>
       <c r="F48" s="19" t="s">
         <v>34</v>
       </c>
@@ -7167,16 +7167,16 @@
     <row r="49" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="117" t="s">
+      <c r="C49" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="118"/>
-      <c r="E49" s="119"/>
+      <c r="D49" s="107"/>
+      <c r="E49" s="108"/>
       <c r="F49" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>73</v>
@@ -7192,9 +7192,9 @@
     <row r="50" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="8"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="100"/>
-      <c r="E50" s="101"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="96"/>
       <c r="F50" s="19"/>
       <c r="G50" s="17"/>
       <c r="H50" s="15"/>
@@ -7209,9 +7209,9 @@
     <row r="51" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="9"/>
-      <c r="C51" s="123"/>
-      <c r="D51" s="124"/>
-      <c r="E51" s="125"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="114"/>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="21"/>
@@ -7225,54 +7225,54 @@
     </row>
     <row r="52" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="3"/>
-      <c r="C52" s="120"/>
-      <c r="D52" s="121"/>
-      <c r="E52" s="122"/>
+      <c r="C52" s="109"/>
+      <c r="D52" s="110"/>
+      <c r="E52" s="111"/>
       <c r="F52" s="17"/>
       <c r="G52" s="22"/>
       <c r="H52" s="4"/>
       <c r="I52" s="7"/>
     </row>
     <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="108" t="s">
+      <c r="B53" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="109"/>
-      <c r="D53" s="109"/>
-      <c r="E53" s="109"/>
-      <c r="F53" s="109"/>
-      <c r="G53" s="109"/>
-      <c r="H53" s="110"/>
+      <c r="C53" s="98"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="98"/>
+      <c r="F53" s="98"/>
+      <c r="G53" s="98"/>
+      <c r="H53" s="99"/>
       <c r="I53" s="24"/>
     </row>
     <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="111"/>
-      <c r="C54" s="112"/>
-      <c r="D54" s="112"/>
-      <c r="E54" s="112"/>
-      <c r="F54" s="112"/>
-      <c r="G54" s="112"/>
-      <c r="H54" s="113"/>
+      <c r="B54" s="100"/>
+      <c r="C54" s="101"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="101"/>
+      <c r="H54" s="102"/>
       <c r="I54" s="24"/>
     </row>
     <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="111"/>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="113"/>
+      <c r="B55" s="100"/>
+      <c r="C55" s="101"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="101"/>
+      <c r="F55" s="101"/>
+      <c r="G55" s="101"/>
+      <c r="H55" s="102"/>
       <c r="I55" s="24"/>
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="114"/>
-      <c r="C56" s="115"/>
-      <c r="D56" s="115"/>
-      <c r="E56" s="115"/>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="116"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="104"/>
+      <c r="D56" s="104"/>
+      <c r="E56" s="104"/>
+      <c r="F56" s="104"/>
+      <c r="G56" s="104"/>
+      <c r="H56" s="105"/>
       <c r="I56" s="24"/>
     </row>
     <row r="57" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -7292,8 +7292,8 @@
       <c r="D58" s="26"/>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
-      <c r="G58" s="82"/>
-      <c r="H58" s="82"/>
+      <c r="G58" s="92"/>
+      <c r="H58" s="92"/>
       <c r="K58" s="47"/>
     </row>
     <row r="59" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -7302,8 +7302,8 @@
       <c r="D59" s="26"/>
       <c r="E59" s="26"/>
       <c r="F59" s="26"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="82"/>
+      <c r="G59" s="92"/>
+      <c r="H59" s="92"/>
       <c r="K59" s="47"/>
     </row>
     <row r="60" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -7312,15 +7312,15 @@
       <c r="D60" s="26"/>
       <c r="E60" s="26"/>
       <c r="F60" s="26"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="82"/>
+      <c r="G60" s="92"/>
+      <c r="H60" s="92"/>
       <c r="K60" s="47"/>
     </row>
     <row r="61" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="82"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="82"/>
+      <c r="B61" s="92"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="92"/>
+      <c r="E61" s="92"/>
       <c r="F61" s="26"/>
       <c r="G61" s="26"/>
       <c r="H61" s="26"/>
@@ -7483,9 +7483,9 @@
     </row>
     <row r="88" spans="2:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B88" s="26"/>
-      <c r="C88" s="80"/>
-      <c r="D88" s="80"/>
-      <c r="E88" s="80"/>
+      <c r="C88" s="91"/>
+      <c r="D88" s="91"/>
+      <c r="E88" s="91"/>
       <c r="F88" s="26"/>
       <c r="G88" s="26"/>
       <c r="H88" s="26"/>
@@ -9721,6 +9721,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G2:H5"/>
+    <mergeCell ref="G58:H60"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="B53:H56"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="B8:B19"/>
@@ -9737,75 +9806,6 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="B53:H56"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G2:H5"/>
-    <mergeCell ref="G58:H60"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G18:H18" location="'Stack-up'!A1" display="See "/>

</xml_diff>